<commit_message>
TD-3202-Delegate activities export to excel implemented.
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Web.Tests/TestData/CourseDelegateExportAllDataDownloadTest.xlsx
+++ b/DigitalLearningSolutions.Web.Tests/TestData/CourseDelegateExportAllDataDownloadTest.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\digitallearningsolutions\DigitalLearningSolutions.Data.Tests\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\DLSMain\DLSV2\DigitalLearningSolutions.Web.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC1E2C1-860C-4241-912C-02864BCADB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8025D6-249C-4CF9-B9FF-478325B1F253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="2835" windowWidth="28996" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Delegates" sheetId="2" r:id="rId1"/>
+    <sheet name="Self Assessment Delegates" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>Last name</t>
   </si>
@@ -152,6 +153,21 @@
   </si>
   <si>
     <t>Course Two - v1</t>
+  </si>
+  <si>
+    <t>Self assessment name</t>
+  </si>
+  <si>
+    <t>PRN</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Signed off</t>
+  </si>
+  <si>
+    <t>Launches</t>
   </si>
 </sst>
 </file>
@@ -209,19 +225,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -263,6 +284,32 @@
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Admin field 1"/>
     <tableColumn id="23" xr3:uid="{04D7AC53-2572-4598-A52E-C298A0B2E3D9}" name="Admin field 2"/>
     <tableColumn id="24" xr3:uid="{FBCB6D49-CBAE-403F-BB25-4A4513C87130}" name="Admin field 3"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8455723-F2B4-47C1-8C61-90F611CFB013}" name="Table2" displayName="Table2" ref="A1:Q2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Self assessment name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Last name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="First name"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Email"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="PRN"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Role type"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Manager"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Base / office / place of work"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Base / office / place of work (Prompt 4)"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Contact telephone number"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Delegate ID"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Enrolled"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Last accessed"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Complete by"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Submitted"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Signed off"/>
+    <tableColumn id="17" xr3:uid="{B129987B-DFFA-42A0-9F11-6B8D77F1C28D}" name="Launches"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -558,38 +605,38 @@
   </sheetPr>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="1" max="2" width="13.26171875" customWidth="1"/>
+    <col min="3" max="3" width="13.5234375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="47.81640625" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
-    <col min="7" max="7" width="28.26953125" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
-    <col min="9" max="9" width="27.54296875" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" customWidth="1"/>
-    <col min="11" max="12" width="19.81640625" customWidth="1"/>
-    <col min="13" max="13" width="15.26953125" customWidth="1"/>
-    <col min="14" max="14" width="19.81640625" customWidth="1"/>
-    <col min="15" max="15" width="9.81640625" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" customWidth="1"/>
-    <col min="17" max="17" width="18.453125" customWidth="1"/>
-    <col min="18" max="18" width="21.7265625" customWidth="1"/>
-    <col min="19" max="19" width="12.26953125" customWidth="1"/>
-    <col min="20" max="20" width="9.81640625" customWidth="1"/>
-    <col min="21" max="21" width="16.81640625" customWidth="1"/>
-    <col min="22" max="22" width="10.54296875" customWidth="1"/>
-    <col min="23" max="23" width="20.81640625" customWidth="1"/>
-    <col min="24" max="24" width="14.26953125" customWidth="1"/>
-    <col min="25" max="25" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="47.7890625" customWidth="1"/>
+    <col min="6" max="6" width="18.26171875" customWidth="1"/>
+    <col min="7" max="7" width="28.26171875" customWidth="1"/>
+    <col min="8" max="8" width="13.7890625" customWidth="1"/>
+    <col min="9" max="9" width="27.5234375" customWidth="1"/>
+    <col min="10" max="10" width="14.47265625" customWidth="1"/>
+    <col min="11" max="12" width="19.7890625" customWidth="1"/>
+    <col min="13" max="13" width="15.26171875" customWidth="1"/>
+    <col min="14" max="14" width="19.7890625" customWidth="1"/>
+    <col min="15" max="15" width="9.7890625" customWidth="1"/>
+    <col min="16" max="16" width="17.47265625" customWidth="1"/>
+    <col min="17" max="17" width="18.47265625" customWidth="1"/>
+    <col min="18" max="18" width="21.734375" customWidth="1"/>
+    <col min="19" max="19" width="12.26171875" customWidth="1"/>
+    <col min="20" max="20" width="9.7890625" customWidth="1"/>
+    <col min="21" max="21" width="16.7890625" customWidth="1"/>
+    <col min="22" max="22" width="10.5234375" customWidth="1"/>
+    <col min="23" max="23" width="20.7890625" customWidth="1"/>
+    <col min="24" max="24" width="14.26171875" customWidth="1"/>
+    <col min="25" max="25" width="11.7890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -666,19 +713,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="3"/>
-      <c r="T2" s="2"/>
-      <c r="V2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -700,14 +745,14 @@
       <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>41053</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>43167</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="2"/>
       <c r="O3">
         <v>2</v>
       </c>
@@ -723,14 +768,14 @@
       <c r="S3">
         <v>0</v>
       </c>
-      <c r="T3" s="2" t="b">
+      <c r="T3" t="b">
         <v>1</v>
       </c>
-      <c r="V3" s="2" t="b">
+      <c r="V3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -752,14 +797,14 @@
       <c r="J4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>40443</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>43167</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="3">
+      <c r="M4" s="3"/>
+      <c r="N4" s="2">
         <v>43167</v>
       </c>
       <c r="O4">
@@ -777,14 +822,14 @@
       <c r="S4">
         <v>100</v>
       </c>
-      <c r="T4" s="2" t="b">
+      <c r="T4" t="b">
         <v>1</v>
       </c>
-      <c r="V4" s="2" t="b">
+      <c r="V4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -806,14 +851,14 @@
       <c r="J5" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>40624</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>43167</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="3">
+      <c r="M5" s="3"/>
+      <c r="N5" s="2">
         <v>43167</v>
       </c>
       <c r="O5">
@@ -831,20 +876,20 @@
       <c r="S5">
         <v>100</v>
       </c>
-      <c r="T5" s="2" t="b">
+      <c r="T5" t="b">
         <v>1</v>
       </c>
-      <c r="V5" s="2" t="b">
+      <c r="V5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -866,14 +911,14 @@
       <c r="J7" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>41053</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>43167</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="2"/>
       <c r="O7">
         <v>2</v>
       </c>
@@ -889,14 +934,14 @@
       <c r="S7">
         <v>0</v>
       </c>
-      <c r="T7" s="2" t="b">
+      <c r="T7" t="b">
         <v>1</v>
       </c>
-      <c r="V7" s="2" t="b">
+      <c r="V7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -918,14 +963,14 @@
       <c r="J8" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>40443</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>43167</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="3">
+      <c r="M8" s="3"/>
+      <c r="N8" s="2">
         <v>43167</v>
       </c>
       <c r="O8">
@@ -943,20 +988,18 @@
       <c r="S8">
         <v>100</v>
       </c>
-      <c r="T8" s="2" t="b">
+      <c r="T8" t="b">
         <v>1</v>
       </c>
-      <c r="V8" s="2" t="b">
+      <c r="V8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="3"/>
-      <c r="T9" s="2"/>
-      <c r="V9" s="2"/>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -970,4 +1013,97 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8F436D-A61C-451F-AB2C-EBD72665F7E3}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="85.7890625" customWidth="1"/>
+    <col min="2" max="2" width="24.3125" customWidth="1"/>
+    <col min="3" max="3" width="23.9453125" customWidth="1"/>
+    <col min="4" max="4" width="31.578125" customWidth="1"/>
+    <col min="5" max="5" width="10.26171875" customWidth="1"/>
+    <col min="6" max="6" width="29.3671875" customWidth="1"/>
+    <col min="7" max="7" width="10.41796875" customWidth="1"/>
+    <col min="8" max="8" width="25.05078125" customWidth="1"/>
+    <col min="9" max="9" width="21.1015625" customWidth="1"/>
+    <col min="10" max="10" width="14.41796875" customWidth="1"/>
+    <col min="11" max="12" width="19.89453125" customWidth="1"/>
+    <col min="13" max="13" width="15.3125" customWidth="1"/>
+    <col min="14" max="15" width="19.89453125" customWidth="1"/>
+    <col min="16" max="16" width="12.47265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>